<commit_message>
Adicao painel de administracao
</commit_message>
<xml_diff>
--- a/files/Funcionarios.xlsx
+++ b/files/Funcionarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\jvfalves\documentos\projetos\chatbot_apontamento_horas\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28A083C-6959-4DDE-AA70-0175F61676A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4560C336-6BA4-45CB-B155-A2500C4F0F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{9B70C42A-D8B4-494D-8EC9-BB39FF86FF5E}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9B70C42A-D8B4-494D-8EC9-BB39FF86FF5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionarios" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="226">
   <si>
     <t>usuario</t>
   </si>
@@ -674,10 +674,49 @@
     <t>Sim</t>
   </si>
   <si>
-    <t>Booker@1010</t>
-  </si>
-  <si>
     <t>nome_gestor</t>
+  </si>
+  <si>
+    <t>DEPARTAMENTO PESSOAL</t>
+  </si>
+  <si>
+    <t>KARINE CASTRO</t>
+  </si>
+  <si>
+    <t>karine.castro@bookerbrasil.com</t>
+  </si>
+  <si>
+    <t>karine.castro</t>
+  </si>
+  <si>
+    <t>Sócio</t>
+  </si>
+  <si>
+    <t>RUDGE RODRIGUES</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>rudge.rodrigues</t>
+  </si>
+  <si>
+    <t>rudge.rodrigues@bookerbrasil.com</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>leandro.santana</t>
+  </si>
+  <si>
+    <t>leandro.santana@bookerbrasil.com</t>
+  </si>
+  <si>
+    <t>LEANDRO SANTANA</t>
+  </si>
+  <si>
+    <t>CONTABIL</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F6ACB45-F5D3-4013-80F4-6C3637B4EDD0}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,10 +1111,10 @@
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1098,7 +1137,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -1108,9 +1147,7 @@
       <c r="A2" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" t="s">
         <v>82</v>
       </c>
@@ -1134,9 +1171,7 @@
       <c r="A3" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" t="s">
         <v>83</v>
       </c>
@@ -1160,9 +1195,7 @@
       <c r="A4" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" t="s">
         <v>84</v>
       </c>
@@ -1186,9 +1219,7 @@
       <c r="A5" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" t="s">
         <v>85</v>
       </c>
@@ -1212,9 +1243,7 @@
       <c r="A6" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" t="s">
         <v>86</v>
       </c>
@@ -1238,9 +1267,7 @@
       <c r="A7" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="C7" t="s">
         <v>87</v>
       </c>
@@ -1264,9 +1291,7 @@
       <c r="A8" t="s">
         <v>147</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="C8" t="s">
         <v>88</v>
       </c>
@@ -1290,9 +1315,7 @@
       <c r="A9" t="s">
         <v>148</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" t="s">
         <v>89</v>
       </c>
@@ -1316,9 +1339,7 @@
       <c r="A10" t="s">
         <v>149</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="C10" t="s">
         <v>90</v>
       </c>
@@ -1342,9 +1363,7 @@
       <c r="A11" t="s">
         <v>150</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B11" s="1"/>
       <c r="C11" t="s">
         <v>91</v>
       </c>
@@ -1368,9 +1387,7 @@
       <c r="A12" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B12" s="1"/>
       <c r="C12" t="s">
         <v>92</v>
       </c>
@@ -1394,9 +1411,7 @@
       <c r="A13" t="s">
         <v>152</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" t="s">
         <v>93</v>
       </c>
@@ -1404,13 +1419,13 @@
         <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F13" t="s">
         <v>208</v>
       </c>
       <c r="G13" t="s">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="H13" t="s">
         <v>210</v>
@@ -1420,9 +1435,7 @@
       <c r="A14" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" t="s">
         <v>94</v>
       </c>
@@ -1446,9 +1459,7 @@
       <c r="A15" t="s">
         <v>154</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="C15" t="s">
         <v>11</v>
       </c>
@@ -1456,13 +1467,13 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F15" t="s">
         <v>208</v>
       </c>
       <c r="G15" t="s">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="H15" t="s">
         <v>210</v>
@@ -1472,9 +1483,7 @@
       <c r="A16" t="s">
         <v>155</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B16" s="1"/>
       <c r="C16" t="s">
         <v>95</v>
       </c>
@@ -1498,9 +1507,7 @@
       <c r="A17" t="s">
         <v>156</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B17" s="1"/>
       <c r="C17" t="s">
         <v>96</v>
       </c>
@@ -1524,9 +1531,7 @@
       <c r="A18" t="s">
         <v>157</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="C18" t="s">
         <v>97</v>
       </c>
@@ -1550,9 +1555,7 @@
       <c r="A19" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="C19" t="s">
         <v>98</v>
       </c>
@@ -1576,9 +1579,7 @@
       <c r="A20" t="s">
         <v>159</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B20" s="1"/>
       <c r="C20" t="s">
         <v>99</v>
       </c>
@@ -1602,9 +1603,7 @@
       <c r="A21" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B21" s="1"/>
       <c r="C21" t="s">
         <v>100</v>
       </c>
@@ -1628,9 +1627,7 @@
       <c r="A22" t="s">
         <v>161</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B22" s="1"/>
       <c r="C22" t="s">
         <v>101</v>
       </c>
@@ -1654,9 +1651,7 @@
       <c r="A23" t="s">
         <v>162</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B23" s="1"/>
       <c r="C23" t="s">
         <v>25</v>
       </c>
@@ -1680,9 +1675,7 @@
       <c r="A24" t="s">
         <v>163</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B24" s="1"/>
       <c r="C24" t="s">
         <v>102</v>
       </c>
@@ -1706,9 +1699,7 @@
       <c r="A25" t="s">
         <v>164</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B25" s="1"/>
       <c r="C25" t="s">
         <v>103</v>
       </c>
@@ -1732,9 +1723,7 @@
       <c r="A26" t="s">
         <v>165</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B26" s="1"/>
       <c r="C26" t="s">
         <v>104</v>
       </c>
@@ -1758,9 +1747,7 @@
       <c r="A27" t="s">
         <v>166</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1768,13 +1755,13 @@
         <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="F27" t="s">
         <v>208</v>
       </c>
       <c r="G27" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="H27" t="s">
         <v>210</v>
@@ -1784,9 +1771,7 @@
       <c r="A28" t="s">
         <v>167</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B28" s="1"/>
       <c r="C28" t="s">
         <v>106</v>
       </c>
@@ -1810,9 +1795,7 @@
       <c r="A29" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B29" s="1"/>
       <c r="C29" t="s">
         <v>107</v>
       </c>
@@ -1836,9 +1819,7 @@
       <c r="A30" t="s">
         <v>169</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B30" s="1"/>
       <c r="C30" t="s">
         <v>108</v>
       </c>
@@ -1846,13 +1827,13 @@
         <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F30" t="s">
         <v>208</v>
       </c>
       <c r="G30" t="s">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="H30" t="s">
         <v>210</v>
@@ -1862,9 +1843,7 @@
       <c r="A31" t="s">
         <v>170</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B31" s="1"/>
       <c r="C31" t="s">
         <v>109</v>
       </c>
@@ -1872,13 +1851,13 @@
         <v>32</v>
       </c>
       <c r="E31" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F31" t="s">
         <v>208</v>
       </c>
       <c r="G31" t="s">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="H31" t="s">
         <v>210</v>
@@ -1888,9 +1867,7 @@
       <c r="A32" t="s">
         <v>171</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B32" s="1"/>
       <c r="C32" t="s">
         <v>110</v>
       </c>
@@ -1914,9 +1891,7 @@
       <c r="A33" t="s">
         <v>172</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B33" s="1"/>
       <c r="C33" t="s">
         <v>50</v>
       </c>
@@ -1940,9 +1915,7 @@
       <c r="A34" t="s">
         <v>173</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B34" s="1"/>
       <c r="C34" t="s">
         <v>111</v>
       </c>
@@ -1966,9 +1939,7 @@
       <c r="A35" t="s">
         <v>174</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B35" s="1"/>
       <c r="C35" t="s">
         <v>112</v>
       </c>
@@ -1992,9 +1963,7 @@
       <c r="A36" t="s">
         <v>175</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B36" s="1"/>
       <c r="C36" t="s">
         <v>113</v>
       </c>
@@ -2018,9 +1987,7 @@
       <c r="A37" t="s">
         <v>176</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B37" s="1"/>
       <c r="C37" t="s">
         <v>105</v>
       </c>
@@ -2044,9 +2011,7 @@
       <c r="A38" t="s">
         <v>177</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B38" s="1"/>
       <c r="C38" t="s">
         <v>114</v>
       </c>
@@ -2070,9 +2035,7 @@
       <c r="A39" t="s">
         <v>178</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B39" s="1"/>
       <c r="C39" t="s">
         <v>115</v>
       </c>
@@ -2096,9 +2059,7 @@
       <c r="A40" t="s">
         <v>179</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B40" s="1"/>
       <c r="C40" t="s">
         <v>116</v>
       </c>
@@ -2122,9 +2083,7 @@
       <c r="A41" t="s">
         <v>180</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B41" s="1"/>
       <c r="C41" t="s">
         <v>117</v>
       </c>
@@ -2148,9 +2107,7 @@
       <c r="A42" t="s">
         <v>181</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B42" s="1"/>
       <c r="C42" t="s">
         <v>118</v>
       </c>
@@ -2174,9 +2131,7 @@
       <c r="A43" t="s">
         <v>182</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B43" s="1"/>
       <c r="C43" t="s">
         <v>13</v>
       </c>
@@ -2200,9 +2155,7 @@
       <c r="A44" t="s">
         <v>183</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B44" s="1"/>
       <c r="C44" t="s">
         <v>119</v>
       </c>
@@ -2226,9 +2179,7 @@
       <c r="A45" t="s">
         <v>184</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B45" s="1"/>
       <c r="C45" t="s">
         <v>120</v>
       </c>
@@ -2252,9 +2203,7 @@
       <c r="A46" t="s">
         <v>185</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B46" s="1"/>
       <c r="C46" t="s">
         <v>121</v>
       </c>
@@ -2278,9 +2227,7 @@
       <c r="A47" t="s">
         <v>186</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B47" s="1"/>
       <c r="C47" t="s">
         <v>44</v>
       </c>
@@ -2304,9 +2251,7 @@
       <c r="A48" t="s">
         <v>187</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B48" s="1"/>
       <c r="C48" t="s">
         <v>122</v>
       </c>
@@ -2314,13 +2259,13 @@
         <v>59</v>
       </c>
       <c r="E48" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F48" t="s">
         <v>208</v>
       </c>
       <c r="G48" t="s">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="H48" t="s">
         <v>210</v>
@@ -2330,9 +2275,7 @@
       <c r="A49" t="s">
         <v>188</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B49" s="1"/>
       <c r="C49" t="s">
         <v>123</v>
       </c>
@@ -2356,9 +2299,7 @@
       <c r="A50" t="s">
         <v>189</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B50" s="1"/>
       <c r="C50" t="s">
         <v>16</v>
       </c>
@@ -2382,9 +2323,7 @@
       <c r="A51" t="s">
         <v>190</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B51" s="1"/>
       <c r="C51" t="s">
         <v>19</v>
       </c>
@@ -2408,9 +2347,7 @@
       <c r="A52" t="s">
         <v>191</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B52" s="1"/>
       <c r="C52" t="s">
         <v>124</v>
       </c>
@@ -2434,9 +2371,7 @@
       <c r="A53" t="s">
         <v>192</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B53" s="1"/>
       <c r="C53" t="s">
         <v>125</v>
       </c>
@@ -2444,13 +2379,13 @@
         <v>39</v>
       </c>
       <c r="E53" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F53" t="s">
         <v>208</v>
       </c>
       <c r="G53" t="s">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="H53" t="s">
         <v>210</v>
@@ -2460,9 +2395,7 @@
       <c r="A54" t="s">
         <v>193</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B54" s="1"/>
       <c r="C54" t="s">
         <v>126</v>
       </c>
@@ -2486,9 +2419,7 @@
       <c r="A55" t="s">
         <v>194</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B55" s="1"/>
       <c r="C55" t="s">
         <v>127</v>
       </c>
@@ -2512,9 +2443,7 @@
       <c r="A56" t="s">
         <v>195</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B56" s="1"/>
       <c r="C56" t="s">
         <v>128</v>
       </c>
@@ -2538,9 +2467,7 @@
       <c r="A57" t="s">
         <v>196</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B57" s="1"/>
       <c r="C57" t="s">
         <v>129</v>
       </c>
@@ -2548,13 +2475,13 @@
         <v>20</v>
       </c>
       <c r="E57" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F57" t="s">
         <v>208</v>
       </c>
       <c r="G57" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H57" t="s">
         <v>210</v>
@@ -2564,9 +2491,7 @@
       <c r="A58" t="s">
         <v>197</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B58" s="1"/>
       <c r="C58" t="s">
         <v>130</v>
       </c>
@@ -2590,9 +2515,7 @@
       <c r="A59" t="s">
         <v>198</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B59" s="1"/>
       <c r="C59" t="s">
         <v>131</v>
       </c>
@@ -2616,9 +2539,7 @@
       <c r="A60" t="s">
         <v>199</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B60" s="1"/>
       <c r="C60" t="s">
         <v>132</v>
       </c>
@@ -2642,9 +2563,7 @@
       <c r="A61" t="s">
         <v>200</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B61" s="1"/>
       <c r="C61" t="s">
         <v>133</v>
       </c>
@@ -2668,9 +2587,7 @@
       <c r="A62" t="s">
         <v>201</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B62" s="1"/>
       <c r="C62" t="s">
         <v>134</v>
       </c>
@@ -2678,13 +2595,13 @@
         <v>74</v>
       </c>
       <c r="E62" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F62" t="s">
         <v>208</v>
       </c>
       <c r="G62" t="s">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="H62" t="s">
         <v>210</v>
@@ -2694,9 +2611,7 @@
       <c r="A63" t="s">
         <v>202</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B63" s="1"/>
       <c r="C63" t="s">
         <v>135</v>
       </c>
@@ -2720,9 +2635,7 @@
       <c r="A64" t="s">
         <v>203</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B64" s="1"/>
       <c r="C64" t="s">
         <v>136</v>
       </c>
@@ -2746,9 +2659,7 @@
       <c r="A65" t="s">
         <v>204</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B65" s="1"/>
       <c r="C65" t="s">
         <v>137</v>
       </c>
@@ -2756,13 +2667,13 @@
         <v>67</v>
       </c>
       <c r="E65" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="F65" t="s">
         <v>208</v>
       </c>
       <c r="G65" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="H65" t="s">
         <v>210</v>
@@ -2772,9 +2683,7 @@
       <c r="A66" t="s">
         <v>205</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B66" s="1"/>
       <c r="C66" t="s">
         <v>138</v>
       </c>
@@ -2798,9 +2707,7 @@
       <c r="A67" t="s">
         <v>206</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B67" s="1"/>
       <c r="C67" t="s">
         <v>139</v>
       </c>
@@ -2824,9 +2731,7 @@
       <c r="A68" t="s">
         <v>207</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="B68" s="1"/>
       <c r="C68" t="s">
         <v>140</v>
       </c>
@@ -2834,37 +2739,96 @@
         <v>42</v>
       </c>
       <c r="E68" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="F68" t="s">
         <v>208</v>
       </c>
       <c r="G68" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="H68" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>215</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D69" t="s">
+        <v>213</v>
+      </c>
+      <c r="E69" t="s">
+        <v>212</v>
+      </c>
+      <c r="F69" t="s">
+        <v>216</v>
+      </c>
+      <c r="H69" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>219</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D70" t="s">
+        <v>217</v>
+      </c>
+      <c r="E70" t="s">
+        <v>221</v>
+      </c>
+      <c r="F70" t="s">
+        <v>216</v>
+      </c>
+      <c r="H70" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>222</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D71" t="s">
+        <v>224</v>
+      </c>
+      <c r="E71" t="s">
+        <v>225</v>
+      </c>
+      <c r="F71" t="s">
+        <v>216</v>
+      </c>
+      <c r="H71" t="s">
         <v>210</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C27" r:id="rId1" xr:uid="{8A8AC972-EC30-49B5-B483-0F27F204A08F}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{2584385E-CACF-4A14-BC24-D1E25F75BE4B}"/>
-    <hyperlink ref="B3:B68" r:id="rId3" display="Booker@1010" xr:uid="{4DC71DAB-65BC-43AD-97C9-B20FD8F0EA33}"/>
+    <hyperlink ref="C69" r:id="rId2" xr:uid="{5C273392-05BE-4417-8373-6B0B72C6BD96}"/>
+    <hyperlink ref="C70" r:id="rId3" xr:uid="{28A67060-AA70-4F7E-B4D8-E29E605FC9BC}"/>
+    <hyperlink ref="C71" r:id="rId4" xr:uid="{0D8C1011-6F4A-44A4-8132-322CEDD991DE}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="312247fe-d295-4069-a5c8-f0300302237f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="96a67299-4560-4510-9370-63b35f134a04">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3057,21 +3021,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="312247fe-d295-4069-a5c8-f0300302237f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="96a67299-4560-4510-9370-63b35f134a04">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EA040A6-54E3-40C6-9725-B92C12A3B30F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C64FE9BE-76A3-403F-99FD-FB199000873E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="312247fe-d295-4069-a5c8-f0300302237f"/>
-    <ds:schemaRef ds:uri="96a67299-4560-4510-9370-63b35f134a04"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3096,9 +3059,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C64FE9BE-76A3-403F-99FD-FB199000873E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EA040A6-54E3-40C6-9725-B92C12A3B30F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="312247fe-d295-4069-a5c8-f0300302237f"/>
+    <ds:schemaRef ds:uri="96a67299-4560-4510-9370-63b35f134a04"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Versao atualizada com dashboard
</commit_message>
<xml_diff>
--- a/files/Funcionarios.xlsx
+++ b/files/Funcionarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\jvfalves\documentos\projetos\chatbot_apontamento_horas\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4560C336-6BA4-45CB-B155-A2500C4F0F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DF8DE4-9701-49F1-8DE5-FB69E0DB2FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9B70C42A-D8B4-494D-8EC9-BB39FF86FF5E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{9B70C42A-D8B4-494D-8EC9-BB39FF86FF5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionarios" sheetId="1" r:id="rId1"/>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F6ACB45-F5D3-4013-80F4-6C3637B4EDD0}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2823,15 +2823,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B0DC5D8F98F30F48A1067D5314F71C8B" ma:contentTypeVersion="10" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="a6c8bf3bda617f979e2cb9cddfcd75a0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="96a67299-4560-4510-9370-63b35f134a04" xmlns:ns3="312247fe-d295-4069-a5c8-f0300302237f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d288853c0c2e4a3e837d50f0b69d60e6" ns2:_="" ns3:_="">
     <xsd:import namespace="96a67299-4560-4510-9370-63b35f134a04"/>
@@ -3020,6 +3011,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3032,14 +3032,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C64FE9BE-76A3-403F-99FD-FB199000873E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1B4D1A1-69FB-4BE5-AF97-714350C0F090}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3058,6 +3050,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C64FE9BE-76A3-403F-99FD-FB199000873E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EA040A6-54E3-40C6-9725-B92C12A3B30F}">
   <ds:schemaRefs>

</xml_diff>